<commit_message>
'Gesellschaften in 'Firmen' umbenannt. Optionale Attribute implemntiert. Code entsprechend angepasst. Alle Tests laufen.
</commit_message>
<xml_diff>
--- a/src/test/testdaten_insert_unfallversicherungsbeitrag/Unfallversicherungsbeitrag - Folgejahr.xlsx
+++ b/src/test/testdaten_insert_unfallversicherungsbeitrag/Unfallversicherungsbeitrag - Folgejahr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_unfallversicherungsbeitrag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E04CDF-7410-45E0-A851-9D7226F94099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EE9544-E626-4A70-8E60-5C7A444E829C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,15 +36,9 @@
     <t>Berufsgenossenschaft</t>
   </si>
   <si>
-    <t>Gesellschaft</t>
-  </si>
-  <si>
     <t>Berufsgenossenschaftskuerzel</t>
   </si>
   <si>
-    <t>Gesellschaftskuerzel</t>
-  </si>
-  <si>
     <t>Jahresbeitrag Unfallversicherung</t>
   </si>
   <si>
@@ -61,6 +55,12 @@
   </si>
   <si>
     <t>BGN</t>
+  </si>
+  <si>
+    <t>Unternehmen</t>
+  </si>
+  <si>
+    <t>Unternehmenskuerzel</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,18 +412,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -431,20 +431,20 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>6748512.3099999996</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>2024</v>

</xml_diff>